<commit_message>
Add tools Labeled Data
</commit_message>
<xml_diff>
--- a/Mapping/VulnerablityMap.xlsx
+++ b/Mapping/VulnerablityMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikahjs/Documents/MyFiles/PhDwork/MultiTagging/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0629424A-D3FC-244C-AD8F-CD3E72431596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500E2D4A-CFF3-0C40-BCA9-A3A065CEBA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17180" activeTab="4" xr2:uid="{7B76C7B8-C702-4BBB-AFE9-C0434D238B79}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17180" activeTab="3" xr2:uid="{7B76C7B8-C702-4BBB-AFE9-C0434D238B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Slither" sheetId="6" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="345">
   <si>
     <t>Vulnerability</t>
   </si>
@@ -974,114 +974,6 @@
     <t>state-visibility</t>
   </si>
   <si>
-    <t>compound-borrowfresh-reentrancy</t>
-  </si>
-  <si>
-    <t>compound-sweeptoken-not-restricted</t>
-  </si>
-  <si>
-    <t>erc20-public-transfer</t>
-  </si>
-  <si>
-    <t>erc20-public-burn</t>
-  </si>
-  <si>
-    <t>erc677-reentrancy</t>
-  </si>
-  <si>
-    <t>erc777-reentrancy</t>
-  </si>
-  <si>
-    <t>erc721-reentrancy</t>
-  </si>
-  <si>
-    <t>erc721-arbitrary-transferfrom</t>
-  </si>
-  <si>
-    <t>gearbox-tokens-path-confusion</t>
-  </si>
-  <si>
-    <t>keeper-network-oracle-manipulation</t>
-  </si>
-  <si>
-    <t>basic-oracle-manipulation</t>
-  </si>
-  <si>
-    <t>redacted-cartel-custom-approval-bug</t>
-  </si>
-  <si>
-    <t>rigoblock-missing-access-control</t>
-  </si>
-  <si>
-    <t>oracle-price-update-not-restricted</t>
-  </si>
-  <si>
-    <t>superfluid-ctx-injection</t>
-  </si>
-  <si>
-    <t>tecra-coin-burnfrom-bug</t>
-  </si>
-  <si>
-    <t>arbitrary-low-level-call</t>
-  </si>
-  <si>
-    <t>sense-missing-oracle-access-control</t>
-  </si>
-  <si>
-    <t>proxy-storage-collision</t>
-  </si>
-  <si>
-    <t>uniswap-callback-not-protected</t>
-  </si>
-  <si>
-    <t>openzeppelin-ecdsa-recover-malleable</t>
-  </si>
-  <si>
-    <t>unrestricted-transferownership</t>
-  </si>
-  <si>
-    <t>msg-value-multicall</t>
-  </si>
-  <si>
-    <t>no-bidi-characters</t>
-  </si>
-  <si>
-    <t>delegatecall-to-arbitrary-address</t>
-  </si>
-  <si>
-    <t>incorrect-use-of-blockhash</t>
-  </si>
-  <si>
-    <t>accessible-selfdestruct</t>
-  </si>
-  <si>
-    <t>no-slippage-check</t>
-  </si>
-  <si>
-    <t>balancer-readonly-reentrancy-getrate</t>
-  </si>
-  <si>
-    <t>balancer-readonly-reentrancy-getpooltokens</t>
-  </si>
-  <si>
-    <t>curve-readonly-reentrancy</t>
-  </si>
-  <si>
-    <t>public-transfer-fees-supporting-tax-tokens</t>
-  </si>
-  <si>
-    <t>olympus-dao-staking-incorrect-call-order</t>
-  </si>
-  <si>
-    <t>compound-precision-loss</t>
-  </si>
-  <si>
-    <t>thirdweb-vulnerability</t>
-  </si>
-  <si>
-    <t>exact-balance-check</t>
-  </si>
-  <si>
     <t>https://github.com/Decurity/semgrep-smart-contracts</t>
   </si>
   <si>
@@ -1091,9 +983,6 @@
     <t>Semgrep</t>
   </si>
   <si>
-    <t>basic-arithmetic-underflow</t>
-  </si>
-  <si>
     <t>integer over/underflow</t>
   </si>
   <si>
@@ -1107,6 +996,120 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>compound_borrowfresh_reentrancy</t>
+  </si>
+  <si>
+    <t>compound_sweeptoken_not_restricted</t>
+  </si>
+  <si>
+    <t>erc20_public_transfer</t>
+  </si>
+  <si>
+    <t>erc20_public_burn</t>
+  </si>
+  <si>
+    <t>erc677_reentrancy</t>
+  </si>
+  <si>
+    <t>erc777_reentrancy</t>
+  </si>
+  <si>
+    <t>erc721_reentrancy</t>
+  </si>
+  <si>
+    <t>erc721_arbitrary_transferfrom</t>
+  </si>
+  <si>
+    <t>gearbox_tokens_path_confusion</t>
+  </si>
+  <si>
+    <t>keeper_network_oracle_manipulation</t>
+  </si>
+  <si>
+    <t>basic_oracle_manipulation</t>
+  </si>
+  <si>
+    <t>redacted_cartel_custom_approval_bug</t>
+  </si>
+  <si>
+    <t>rigoblock_missing_access_control</t>
+  </si>
+  <si>
+    <t>oracle_price_update_not_restricted</t>
+  </si>
+  <si>
+    <t>superfluid_ctx_injection</t>
+  </si>
+  <si>
+    <t>tecra_coin_burnfrom_bug</t>
+  </si>
+  <si>
+    <t>arbitrary_low_level_call</t>
+  </si>
+  <si>
+    <t>sense_missing_oracle_access_control</t>
+  </si>
+  <si>
+    <t>proxy_storage_collision</t>
+  </si>
+  <si>
+    <t>uniswap_callback_not_protected</t>
+  </si>
+  <si>
+    <t>encode_packed_collision</t>
+  </si>
+  <si>
+    <t>openzeppelin_ecdsa_recover_malleable</t>
+  </si>
+  <si>
+    <t>basic_arithmetic_underflow</t>
+  </si>
+  <si>
+    <t>unrestricted_transferownership</t>
+  </si>
+  <si>
+    <t>msg_value_multicall</t>
+  </si>
+  <si>
+    <t>no_bidi_characters</t>
+  </si>
+  <si>
+    <t>delegatecall_to_arbitrary_address</t>
+  </si>
+  <si>
+    <t>incorrect_use_of_blockhash</t>
+  </si>
+  <si>
+    <t>accessible_selfdestruct</t>
+  </si>
+  <si>
+    <t>no_slippage_check</t>
+  </si>
+  <si>
+    <t>balancer_readonly_reentrancy_getrate</t>
+  </si>
+  <si>
+    <t>balancer_readonly_reentrancy_getpooltokens</t>
+  </si>
+  <si>
+    <t>curve_readonly_reentrancy</t>
+  </si>
+  <si>
+    <t>public_transfer_fees_supporting_tax_tokens</t>
+  </si>
+  <si>
+    <t>olympus_dao_staking_incorrect_call_order</t>
+  </si>
+  <si>
+    <t>compound_precision_loss</t>
+  </si>
+  <si>
+    <t>thirdweb_vulnerability</t>
+  </si>
+  <si>
+    <t>exact_balance_check</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1163,6 +1166,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1177,7 +1186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1190,6 +1199,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2712,13 +2722,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
       <c r="B8" t="s">
-        <v>337</v>
+        <v>301</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -3326,8 +3336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F92A7D-7178-499D-BCAD-ADC94621388E}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3360,7 +3370,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C2">
         <v>107</v>
@@ -3380,7 +3390,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="C3">
         <v>105</v>
@@ -3400,7 +3410,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3408,7 +3418,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3416,7 +3426,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C6">
         <v>107</v>
@@ -3436,7 +3446,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="C7">
         <v>107</v>
@@ -3456,7 +3466,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C8">
         <v>107</v>
@@ -3476,7 +3486,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3484,7 +3494,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3492,7 +3502,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="C11">
         <v>101</v>
@@ -3512,7 +3522,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="C12">
         <v>101</v>
@@ -3532,7 +3542,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3540,7 +3550,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -3554,7 +3564,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -3568,7 +3578,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>313</v>
+        <v>321</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3576,7 +3586,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3584,7 +3594,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>315</v>
+        <v>323</v>
       </c>
       <c r="C18">
         <v>112</v>
@@ -3593,18 +3603,16 @@
         <v>213</v>
       </c>
       <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18" t="s">
-        <v>213</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>316</v>
+        <v>324</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -3618,7 +3626,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>317</v>
+        <v>325</v>
       </c>
       <c r="C20">
         <v>124</v>
@@ -3638,7 +3646,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>318</v>
+        <v>326</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3646,7 +3654,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>327</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -3654,7 +3662,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C23">
         <v>117</v>
@@ -3674,7 +3682,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="C24">
         <v>101</v>
@@ -3694,7 +3702,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -3708,7 +3716,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3716,7 +3724,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="C27">
         <v>130</v>
@@ -3730,7 +3738,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
       <c r="C28">
         <v>112</v>
@@ -3739,18 +3747,16 @@
         <v>213</v>
       </c>
       <c r="E28">
-        <v>10</v>
-      </c>
-      <c r="F28" t="s">
-        <v>213</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>324</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -3758,7 +3764,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="C30">
         <v>106</v>
@@ -3778,7 +3784,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -3786,7 +3792,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C32">
         <v>107</v>
@@ -3806,7 +3812,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="C33">
         <v>107</v>
@@ -3826,7 +3832,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="C34">
         <v>107</v>
@@ -3846,7 +3852,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3854,7 +3860,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -3862,7 +3868,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -3870,7 +3876,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -3878,7 +3884,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
@@ -3895,7 +3901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C283EE1A-CA87-472E-B6B2-7DC97A7C5B80}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -4080,7 +4086,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>339</v>
+        <v>302</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -4094,7 +4100,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="C3">
         <v>101</v>
@@ -4108,7 +4114,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>341</v>
+        <v>304</v>
       </c>
       <c r="C4">
         <v>106</v>
@@ -4122,7 +4128,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>342</v>
+        <v>305</v>
       </c>
       <c r="C5">
         <v>105</v>
@@ -4146,8 +4152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A642EC6D-AA27-4FDC-A28F-3545E59FFB76}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G38"/>
+    <sheetView topLeftCell="C1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5170,7 +5176,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>343</v>
+        <v>306</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Update mapper and add evaluator_v2
</commit_message>
<xml_diff>
--- a/Mapping/VulnerablityMap.xlsx
+++ b/Mapping/VulnerablityMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shikahjs/Documents/MyFiles/PhDwork/MultiTagging/Mapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C17142-4CF8-3545-8131-70B0B020FBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDFA586-9688-E147-ADC2-47C15F8442BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17180" activeTab="1" xr2:uid="{7B76C7B8-C702-4BBB-AFE9-C0434D238B79}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17180" activeTab="4" xr2:uid="{7B76C7B8-C702-4BBB-AFE9-C0434D238B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Slither" sheetId="6" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="351">
   <si>
     <t>Vulnerability</t>
   </si>
@@ -722,18 +722,6 @@
   </si>
   <si>
     <t>Destructible</t>
-  </si>
-  <si>
-    <t>Destructible (verified)</t>
-  </si>
-  <si>
-    <t>Ether leak</t>
-  </si>
-  <si>
-    <t>Ether leak (verified)</t>
-  </si>
-  <si>
-    <t>Ether lock</t>
   </si>
   <si>
     <t>Ether lock (Ether accepted without send)</t>
@@ -1122,6 +1110,24 @@
   </si>
   <si>
     <t>SWC-127</t>
+  </si>
+  <si>
+    <t>105? 2?</t>
+  </si>
+  <si>
+    <t>120? 6?</t>
+  </si>
+  <si>
+    <t>Ether_leak_verified</t>
+  </si>
+  <si>
+    <t>Destructible_verified</t>
+  </si>
+  <si>
+    <t>Ether_leak</t>
+  </si>
+  <si>
+    <t>Ether_lock</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1184,6 +1190,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1198,7 +1216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1212,6 +1230,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1590,17 +1610,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D15B12-FED7-477E-BE07-615F6A778B56}">
-  <dimension ref="A1:F93"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A46" zoomScale="108" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1636,8 +1657,15 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>120</v>
+      </c>
+      <c r="C3" s="10">
+        <v>105</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1742,14 +1770,14 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>131</v>
       </c>
       <c r="C14">
-        <v>109</v>
-      </c>
-      <c r="D14" t="s">
-        <v>213</v>
+        <v>124</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1786,16 +1814,30 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="10" t="s">
         <v>135</v>
+      </c>
+      <c r="C18" s="10">
+        <v>105</v>
+      </c>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="10" t="s">
         <v>136</v>
+      </c>
+      <c r="C19" s="10">
+        <v>105</v>
+      </c>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -1862,8 +1904,14 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>143</v>
+      </c>
+      <c r="C26">
+        <v>107</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1889,6 +1937,12 @@
       <c r="B29" t="s">
         <v>146</v>
       </c>
+      <c r="C29">
+        <v>104</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1897,6 +1951,12 @@
       <c r="B30" t="s">
         <v>147</v>
       </c>
+      <c r="C30">
+        <v>120</v>
+      </c>
+      <c r="E30">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1942,10 +2002,10 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="8">
         <v>5</v>
       </c>
       <c r="F36" t="s">
@@ -2085,6 +2145,12 @@
       <c r="B49" t="s">
         <v>166</v>
       </c>
+      <c r="C49">
+        <v>104</v>
+      </c>
+      <c r="E49">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
@@ -2093,6 +2159,12 @@
       <c r="B50" t="s">
         <v>167</v>
       </c>
+      <c r="C50">
+        <v>104</v>
+      </c>
+      <c r="E50">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
@@ -2224,8 +2296,15 @@
       <c r="A63">
         <v>62</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="10" t="s">
         <v>180</v>
+      </c>
+      <c r="C63" s="10">
+        <v>105</v>
+      </c>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -2248,15 +2327,21 @@
         <v>213</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="8" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C65">
+        <v>107</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2264,11 +2349,11 @@
         <v>183</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="9" t="s">
         <v>184</v>
       </c>
       <c r="C67">
@@ -2283,8 +2368,11 @@
       <c r="F67" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2292,7 +2380,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2300,7 +2388,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2308,7 +2396,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2316,7 +2404,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2324,7 +2412,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2332,7 +2420,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2340,7 +2428,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2348,7 +2436,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2368,7 +2456,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2376,7 +2464,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2384,7 +2472,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2398,7 +2486,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2406,7 +2494,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2414,7 +2502,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2422,7 +2510,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2436,7 +2524,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2444,7 +2532,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2452,15 +2540,24 @@
         <v>202</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="8" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C86">
+        <v>107</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+      <c r="F86" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2468,7 +2565,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2476,7 +2573,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2484,7 +2581,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2492,7 +2589,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2500,7 +2597,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2508,7 +2605,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2674,7 +2771,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2701,46 +2798,46 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="96" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B8" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -2763,8 +2860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701418C2-0B0F-4393-9AFB-5F5D821ADFF5}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2782,7 +2879,7 @@
         <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>117</v>
@@ -2805,22 +2902,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D2">
         <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F2" s="7">
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -2829,22 +2926,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="D3">
         <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F3" s="7">
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I3" s="1"/>
     </row>
@@ -2853,22 +2950,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C4" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D4">
         <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F4" s="7">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -2877,22 +2974,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D5">
         <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F5" s="7">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -2901,22 +2998,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C6" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D6">
         <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F6" s="7">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -2925,22 +3022,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D7">
         <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F7" s="7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -2949,20 +3046,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C8" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D8">
         <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -2971,20 +3068,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D9">
         <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I9" s="1"/>
     </row>
@@ -2993,20 +3090,20 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C10" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="D10">
         <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I10" s="1"/>
     </row>
@@ -3015,22 +3112,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C11" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="D11">
         <v>113</v>
       </c>
       <c r="E11" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F11" s="7">
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I11" s="1"/>
     </row>
@@ -3039,22 +3136,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C12" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="D12">
         <v>116</v>
       </c>
       <c r="E12" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F12" s="7">
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I12" s="1"/>
     </row>
@@ -3063,22 +3160,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C13" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="D13">
         <v>120</v>
       </c>
       <c r="E13" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F13" s="7">
         <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I13" s="1"/>
     </row>
@@ -3087,22 +3184,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C14" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D14">
         <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F14" s="7">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I14" s="1"/>
     </row>
@@ -3111,20 +3208,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="D15">
         <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="I15" s="1"/>
     </row>
@@ -3177,7 +3274,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3185,7 +3282,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C3">
         <v>104</v>
@@ -3199,7 +3296,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C4">
         <v>106</v>
@@ -3213,7 +3310,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3221,7 +3318,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3229,7 +3326,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C7">
         <v>115</v>
@@ -3243,7 +3340,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3251,7 +3348,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3259,7 +3356,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3267,7 +3364,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -3275,7 +3372,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -3283,7 +3380,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3291,7 +3388,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -3299,7 +3396,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -3307,7 +3404,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C16">
         <v>116</v>
@@ -3321,7 +3418,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C17">
         <v>107</v>
@@ -3335,7 +3432,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -3348,7 +3445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F92A7D-7178-499D-BCAD-ADC94621388E}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="150" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -3382,7 +3479,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C2">
         <v>107</v>
@@ -3402,7 +3499,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C3">
         <v>105</v>
@@ -3422,7 +3519,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -3430,7 +3527,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3438,7 +3535,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C6">
         <v>107</v>
@@ -3458,7 +3555,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C7">
         <v>107</v>
@@ -3478,7 +3575,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C8">
         <v>107</v>
@@ -3498,7 +3595,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3506,7 +3603,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -3514,7 +3611,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C11">
         <v>101</v>
@@ -3534,7 +3631,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C12">
         <v>101</v>
@@ -3554,7 +3651,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3562,7 +3659,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -3576,7 +3673,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -3590,7 +3687,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3598,7 +3695,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3606,7 +3703,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C18">
         <v>112</v>
@@ -3624,7 +3721,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E19">
         <v>2</v>
@@ -3638,7 +3735,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C20">
         <v>124</v>
@@ -3658,7 +3755,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3666,7 +3763,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -3674,7 +3771,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C23">
         <v>117</v>
@@ -3686,7 +3783,7 @@
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3694,7 +3791,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C24">
         <v>101</v>
@@ -3714,7 +3811,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -3728,7 +3825,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3736,7 +3833,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C27">
         <v>130</v>
@@ -3750,7 +3847,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C28">
         <v>112</v>
@@ -3768,7 +3865,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -3776,7 +3873,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C30">
         <v>106</v>
@@ -3796,7 +3893,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -3804,7 +3901,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C32">
         <v>107</v>
@@ -3824,7 +3921,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C33">
         <v>107</v>
@@ -3844,7 +3941,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C34">
         <v>107</v>
@@ -3864,7 +3961,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -3872,7 +3969,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -3880,7 +3977,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -3888,7 +3985,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -3896,7 +3993,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -3911,10 +4008,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C283EE1A-CA87-472E-B6B2-7DC97A7C5B80}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3968,7 +4065,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>348</v>
       </c>
       <c r="C3">
         <v>106</v>
@@ -3988,7 +4085,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>349</v>
       </c>
       <c r="C4">
         <v>105</v>
@@ -4008,7 +4105,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>347</v>
       </c>
       <c r="C5">
         <v>105</v>
@@ -4028,7 +4125,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>350</v>
       </c>
       <c r="E6">
         <v>5</v>
@@ -4042,13 +4139,18 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -4102,10 +4204,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D2">
         <v>101</v>
@@ -4119,10 +4221,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="D3">
         <v>101</v>
@@ -4136,10 +4238,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D4">
         <v>106</v>
@@ -4153,10 +4255,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="D5">
         <v>105</v>
@@ -4180,8 +4282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A642EC6D-AA27-4FDC-A28F-3545E59FFB76}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="B1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4252,10 +4354,10 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4281,7 +4383,7 @@
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K3" t="s">
         <v>112</v>
@@ -4307,10 +4409,10 @@
         <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -4330,10 +4432,10 @@
         <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -4359,7 +4461,7 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K6" t="s">
         <v>112</v>
@@ -4391,7 +4493,7 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J7" t="s">
         <v>114</v>
@@ -4423,7 +4525,7 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J8" t="s">
         <v>116</v>
@@ -4458,7 +4560,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K9" t="s">
         <v>112</v>
@@ -4484,10 +4586,10 @@
         <v>46</v>
       </c>
       <c r="H10" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I10" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -4504,10 +4606,10 @@
         <v>47</v>
       </c>
       <c r="H11" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I11" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L11" t="s">
         <v>112</v>
@@ -4530,10 +4632,10 @@
         <v>48</v>
       </c>
       <c r="H12" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K12" t="s">
         <v>112</v>
@@ -4559,10 +4661,10 @@
         <v>49</v>
       </c>
       <c r="H13" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I13" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -4585,7 +4687,7 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K14" t="s">
         <v>112</v>
@@ -4617,7 +4719,7 @@
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="J15" t="s">
         <v>115</v>
@@ -4646,7 +4748,7 @@
         <v>7</v>
       </c>
       <c r="I16" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K16" t="s">
         <v>112</v>
@@ -4672,7 +4774,7 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L17" t="s">
         <v>112</v>
@@ -4698,7 +4800,7 @@
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="K18" t="s">
         <v>112</v>
@@ -4727,7 +4829,7 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -4750,7 +4852,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -4770,10 +4872,10 @@
         <v>58</v>
       </c>
       <c r="H21" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I21" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -4796,7 +4898,7 @@
         <v>6</v>
       </c>
       <c r="I22" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L22" t="s">
         <v>112</v>
@@ -4819,7 +4921,7 @@
         <v>60</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -4839,7 +4941,7 @@
         <v>61</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -4859,10 +4961,10 @@
         <v>62</v>
       </c>
       <c r="H25" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I25" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -4885,7 +4987,7 @@
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L26" t="s">
         <v>112</v>
@@ -4908,10 +5010,10 @@
         <v>64</v>
       </c>
       <c r="H27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I27" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -4931,7 +5033,7 @@
         <v>65</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -4951,10 +5053,10 @@
         <v>66</v>
       </c>
       <c r="H29" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I29" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L29" t="s">
         <v>112</v>
@@ -4983,7 +5085,7 @@
         <v>5</v>
       </c>
       <c r="I30" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L30" t="s">
         <v>112</v>
@@ -5006,10 +5108,10 @@
         <v>68</v>
       </c>
       <c r="H31" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I31" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -5029,10 +5131,10 @@
         <v>69</v>
       </c>
       <c r="H32" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I32" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -5052,10 +5154,10 @@
         <v>70</v>
       </c>
       <c r="H33" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I33" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -5075,10 +5177,10 @@
         <v>71</v>
       </c>
       <c r="H34" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I34" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -5098,10 +5200,10 @@
         <v>72</v>
       </c>
       <c r="H35" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I35" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -5124,7 +5226,7 @@
         <v>5</v>
       </c>
       <c r="I36" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="L36" t="s">
         <v>112</v>
@@ -5147,10 +5249,10 @@
         <v>74</v>
       </c>
       <c r="H37" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I37" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -5170,10 +5272,10 @@
         <v>75</v>
       </c>
       <c r="H38" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="I38" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -5204,7 +5306,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B1" t="s">
         <v>29</v>
@@ -5516,7 +5618,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5530,16 +5632,16 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="D1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="1"/>
@@ -5552,10 +5654,10 @@
         <v>45</v>
       </c>
       <c r="C2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -5563,10 +5665,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -5574,10 +5676,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5585,10 +5687,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5596,10 +5698,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -5607,10 +5709,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -5618,10 +5720,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -5629,10 +5731,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C9" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -5640,10 +5742,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -5651,7 +5753,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>